<commit_message>
make interval function di sisi mahasiswa saat menampilan data absensi
</commit_message>
<xml_diff>
--- a/excel/format_importdatauser.xlsx
+++ b/excel/format_importdatauser.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\absensi_client\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\absensi_client\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
@@ -479,7 +479,7 @@
   <dimension ref="A1:K90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>